<commit_message>
v0.1: Add arrows in maze_drawer.json.
</commit_message>
<xml_diff>
--- a/rsc/maze.xlsx
+++ b/rsc/maze.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t xml:space="preserve">Start</t>
   </si>
@@ -29,13 +29,64 @@
     <t xml:space="preserve">Bonus</t>
   </si>
   <si>
+    <t xml:space="preserve">TL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replay</t>
+  </si>
+  <si>
     <t xml:space="preserve">Finish</t>
   </si>
   <si>
-    <t xml:space="preserve">Replay</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVBOU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVBOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVBOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVBOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOBU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOBL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COBU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COBL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VBU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VBL</t>
   </si>
   <si>
     <t xml:space="preserve">S</t>
@@ -200,19 +251,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,50 +292,99 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.9296875" defaultRowHeight="38.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.9296875" defaultRowHeight="39.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="7.92"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D6" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" s="9" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -316,7 +416,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -324,23 +424,23 @@
     </row>
     <row r="4" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="s">
-        <v>8</v>
+      <c r="B5" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.2: Square can have a background.
</commit_message>
<xml_diff>
--- a/rsc/maze.xlsx
+++ b/rsc/maze.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="maba" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="maca" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="maze" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="background" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t xml:space="preserve">Start</t>
   </si>
@@ -89,24 +89,7 @@
     <t xml:space="preserve">VBL</t>
   </si>
   <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TR
-OB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LTR
-BGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T</t>
+    <t xml:space="preserve">bg</t>
   </si>
 </sst>
 </file>
@@ -154,7 +137,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -194,13 +177,6 @@
       <left/>
       <right style="medium"/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -230,7 +206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -268,10 +244,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -294,8 +266,8 @@
   </sheetPr>
   <dimension ref="B2:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.9296875" defaultRowHeight="39.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -403,46 +375,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.9296875" defaultRowHeight="38.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.9296875" defaultRowHeight="39.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="7.92"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C3" s="10"/>
-    </row>
-    <row r="4" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
v0.6: Walls can have a color.
</commit_message>
<xml_diff>
--- a/rsc/maze.xlsx
+++ b/rsc/maze.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="maze" sheetId="1" state="visible" r:id="rId2"/>
@@ -137,7 +137,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -147,7 +147,9 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="hair"/>
+      <right style="hair">
+        <color rgb="FF2A6099"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -156,6 +158,13 @@
       <left style="hair"/>
       <right/>
       <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -206,7 +215,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -227,11 +236,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -239,11 +252,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,6 +269,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF2A6099"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -266,8 +339,8 @@
   </sheetPr>
   <dimension ref="B2:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.9296875" defaultRowHeight="39.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -285,12 +358,12 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -299,21 +372,21 @@
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -324,15 +397,15 @@
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -377,7 +450,7 @@
   </sheetPr>
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>